<commit_message>
mintPull Progress made, some planning needs to be done
</commit_message>
<xml_diff>
--- a/test/mintTest.xlsx
+++ b/test/mintTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\AutoMint\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AutoMint\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99232BE5-A9D4-4626-AF9E-D65B3ED5AEE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA525709-FC32-4FC7-AB2C-79A837EDD869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-7290" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6010" yWindow="800" windowWidth="11640" windowHeight="8830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LifeTime_transactions" sheetId="1" r:id="rId1"/>
@@ -954,21 +954,21 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="D2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="21.7265625" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -997,7 +997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44125</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44125</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44125</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44125</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44124</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44123</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44123</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44123</v>
       </c>

</xml_diff>